<commit_message>
fixed error in COP calculation in input file
</commit_message>
<xml_diff>
--- a/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car_extreme_1.xlsx
+++ b/src/pv_optimizer_contracting/data_input_one_month_one_household_one_car_extreme_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\Desktop\DA\Code\pv_optimizer_contracting\src\pv_optimizer_contracting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69B1A24-FECF-4C65-95E7-2BF767FCBC48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950B57E3-FFD4-4D6E-998A-053BFF3CF0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="3" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{A79E091E-0448-41B6-BCFB-F25C6EC10C06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sets" sheetId="10" r:id="rId1"/>
@@ -7870,8 +7870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952F9C99-337E-41EB-9696-FC2C879F8079}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8218,7 +8218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429933C5-DFD0-42DC-9288-AD78420EFB5D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>